<commit_message>
Update MRZ Patolu metadata
</commit_message>
<xml_diff>
--- a/automation/mrz/Meta_Patolu.xlsx
+++ b/automation/mrz/Meta_Patolu.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sszods\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\opendatazurich.github.io\automation\mrz\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-45" windowWidth="21225" windowHeight="12540"/>
+    <workbookView xWindow="20" yWindow="-50" windowWidth="21230" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="14" r:id="rId1"/>
@@ -21,12 +21,12 @@
   <definedNames>
     <definedName name="kategorien" localSheetId="1">kategorien_werteliste!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="230">
   <si>
     <t>Erstmalige Veröffentlichung</t>
   </si>
@@ -997,9 +997,6 @@
     <t>Museum Rietberg Zürich, Präsidialdepartement</t>
   </si>
   <si>
-    <t>Urheber/in des Werks</t>
-  </si>
-  <si>
     <t>Geografische Bezüge</t>
   </si>
   <si>
@@ -1027,150 +1024,202 @@
     <t>Material / Technik</t>
   </si>
   <si>
-    <t>Literatur</t>
-  </si>
-  <si>
-    <t>Bildunterschrift</t>
-  </si>
-  <si>
     <t>Kurzbeschreibung</t>
   </si>
   <si>
-    <t>**Publikation zu Patolu aus Indien**</t>
-  </si>
-  <si>
-    <t>**Museum Rietberg**</t>
-  </si>
-  <si>
-    <t>**Sammlung Online**</t>
-  </si>
-  <si>
-    <t>**Nutzung Bildmaterial**</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
+    <t>Informationen zum Museum Rietberg finden Sie auf der [Webseite](https://rietberg.ch/) des Museums.</t>
+  </si>
+  <si>
+    <t>inventar_nummer</t>
+  </si>
+  <si>
+    <t>bezeichnung</t>
+  </si>
+  <si>
+    <t>urheber</t>
+  </si>
+  <si>
+    <t>geo</t>
+  </si>
+  <si>
+    <t>datum</t>
+  </si>
+  <si>
+    <t>masse</t>
+  </si>
+  <si>
+    <t>material_technik</t>
+  </si>
+  <si>
+    <t>sammlung</t>
+  </si>
+  <si>
+    <t>creditline</t>
+  </si>
+  <si>
+    <t>provenienz</t>
+  </si>
+  <si>
+    <t>kurzbeschreibung</t>
+  </si>
+  <si>
+    <t>bildunterschrift</t>
+  </si>
+  <si>
+    <t>literatur</t>
+  </si>
+  <si>
+    <t>Dateiname</t>
+  </si>
+  <si>
+    <t>Urheber/in</t>
+  </si>
+  <si>
+    <t>Das Museum Rietberg ist das einzige Museum für aussereuropäische Kunst in der Schweiz. Die international renommierte Sammlung beherbergt bedeutende Werke aus Asien, Afrika, Amerika und Ozeanien.
+Einen wesentlichen Bereich der Südasien-Sammlungen bildet die umfassende Textilsammlung (über 2000 Objekte) des ehemaligen Direktors und Indien-Kurators Eberhard Fischer. Er hatte diese während seiner mehrjährigen Aufenthalte in Gujarat, Indien, in den Jahren 1965/66 und 1968–1971 zusammengetragen. 
+Zur Sammlung indischer Textilien zählen auch die hier vorgestellten, besonders wertvollen Patolu, die mehrheitlich Anfang des 20. Jahrhunderts in Gujarat angefertigt wurden. Diese indischen Seidensaris wurden in der sogenannten Doppel-Ikat-Technik gewebt und zeigen typische Motive und Formen wie beispielsweise Blüten und Blätter, geometrische Formen, Tiere und Menschen.
+Bei Doppel-Ikat-Geweben entstehen die Motive und Dekore durch die aufeinander abgestimmte Einfärbung sowohl der Kett- als auch der Schussfäden. Die Fäden werden bereits vor der weiteren Verarbeitung im Webstuhl eingefärbt, wobei die Teile des Fadens, die nicht eingefärbt werden sollen, reserviert, also abgebunden werden.</t>
+  </si>
+  <si>
+    <t>Weiterführende Informationen</t>
+  </si>
+  <si>
+    <t>Museum Rietberg</t>
+  </si>
+  <si>
+    <t>Sammlung Online</t>
+  </si>
+  <si>
+    <t>Bildmaterial</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>**Publikation zu Patolu aus Indien**</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="10"/>
         <color theme="3" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Das Museum Rietberg ist das einzige Museum für aussereuropäische Kunst in der Schweiz. Die international renommierte Sammlung beherbergt bedeutende Werke aus Asien, Afrika, Amerika und Ozeanien.
-Einen wesentlichen Bereich der Südasien-Sammlungen bildet die umfassende Textilsammlung (über 2000 Objekte) des ehemaligen Direktors und Indien-Kurators Eberhard Fischer. Er hatte diese während seiner mehrjährigen Aufenthalte in Gujarat, Indien, in den Jahren 1965/66 und 1968–1971 zusammengetragen. 
-Zur Sammlung indischer Textilien zählen auch die hier vorgestellten, besonders wertvollen Patolu, die mehrheitlich Anfang des 20. Jahrhunderts in Gujarat angefertigt wurden. Diese indischen Seidensaris wurden in der sogenannten Doppel-Ikat-Technik gewebt und zeigen typische Motive und Formen wie beispielsweise Blüten und Blätter, geometrische Formen, Tiere und Menschen.
-Getragen wurden die Seidensaris von </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
+      <t xml:space="preserve">
+Bühler, Alfred und Eberhard Fischer. The Patola of Gujarat: Double Ikat in India. 1979. Basel: Krebs.
+</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">XY zu XY </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>**Die Textilien-Sammlung Eberhard Fischer**</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="10"/>
         <color theme="3" tint="-0.249977111117893"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Anlässen.</t>
-    </r>
-  </si>
-  <si>
-    <t>Bühler, Alfred und Eberhard Fischer. The patola of Gujarat: Double ikat in India. Basel: Krebs, 1979.</t>
-  </si>
-  <si>
-    <t>Informationen zum Museum Rietberg finden Sie auf der [Webseite](https://rietberg.ch/) des Museums.</t>
-  </si>
-  <si>
-    <t>Entdecken Sie weitere Kunstwerke des Museums Reitberg in der [Sammlung Online](https://rietberg.ch/sammlung/sammlung-online).</t>
-  </si>
-  <si>
-    <t>Bildmaterial von Sammlungswerken des Museums Rietberg darf zu nicht-kommerziellen Zwecken genutzt werden. Jede kommerzielle Nutzung von Bildmaterial von Sammlungswerken des Museums Rietberg bedarf einer ausdrücklichen Genehmigung durch das Museum Rietberg und/oder eines entsprechenden, gegenseitig unterschriebenen Vertrags. Wenden Sie sich per [E-Mail] (mailto:medien.rietberg@zuerich.ch) an das Museum Rietberg.</t>
-  </si>
-  <si>
-    <t>inventar_nummer</t>
-  </si>
-  <si>
-    <t>bezeichnung</t>
-  </si>
-  <si>
-    <t>urheber</t>
-  </si>
-  <si>
-    <t>geo</t>
-  </si>
-  <si>
-    <t>datum</t>
-  </si>
-  <si>
-    <t>masse</t>
-  </si>
-  <si>
-    <t>material_technik</t>
-  </si>
-  <si>
-    <t>sammlung</t>
-  </si>
-  <si>
-    <t>creditline</t>
-  </si>
-  <si>
-    <t>provenienz</t>
-  </si>
-  <si>
-    <t>kurzbeschreibung</t>
-  </si>
-  <si>
-    <t>bildunterschrift</t>
-  </si>
-  <si>
-    <t>literatur</t>
-  </si>
-  <si>
-    <t>Dateiname</t>
-  </si>
-  <si>
-    <t>Name der Datei in der ZIP-Datei</t>
-  </si>
-  <si>
-    <t>Inventarnummer im Quellsystem</t>
-  </si>
-  <si>
-    <t>Bezeichnung des Werkes</t>
-  </si>
-  <si>
-    <t>Urheber/in</t>
-  </si>
-  <si>
-    <t>Geografische Bezüge des Werks</t>
-  </si>
-  <si>
-    <t>Datierung des Werks</t>
-  </si>
-  <si>
-    <t>Masse (Lange und Breite)</t>
-  </si>
-  <si>
-    <t>Provenienz (Herkunft)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wissenschaftliche Kurzbeschreibung </t>
-  </si>
-  <si>
-    <t>Literatur-Verweis</t>
-  </si>
-  <si>
-    <t>Quellenangabe</t>
+      <t xml:space="preserve">
+Museum Rietberg Zürich (Hrsg.). [Jahresbericht](https://rietberg.ch/files/Downloads/Jahresbericht/JB09_MRZ.pdf). 2009.  Zürich: Museum Rietberg. S. 48–66.
+Museum Rietberg Zürich (Hrsg.). [Jahresbericht](https://rietberg.ch/files/Downloads/Jahresbericht/JB12_MRZ.pdf). 2012.  Zürich: Museum Rietberg. S. 44–51.</t>
+    </r>
+  </si>
+  <si>
+    <t>Entdecken Sie weitere Kunstwerke des Museums Rietberg in der [Sammlung Online](https://rietberg.ch/sammlung/sammlung-online).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sie möchten eines der Bilder in einer besseren Auflösung nutzen? Dann wenden Sie sich per </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="7" tint="0.59999389629810485"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">[E-Mail](mailto:medien.rietberg@zuerich.ch) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="3" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>direkt an das Museum Rietberg.</t>
+    </r>
+  </si>
+  <si>
+    <t>Literaturverweis</t>
+  </si>
+  <si>
+    <t>Bildnachweis</t>
+  </si>
+  <si>
+    <t>credits</t>
+  </si>
+  <si>
+    <t>Credits</t>
+  </si>
+  <si>
+    <t>Copyrightvermerk des Museums Rietberg, welcher bei der Weiternutzung der Daten verwendet werden muss.</t>
+  </si>
+  <si>
+    <t>Die Inventarnummer dient der eindeutigen Identifikation des Kunstwerks innerhalb der Sammlung des Museums Rietberg.</t>
+  </si>
+  <si>
+    <t>Die Bezeichnung ist ein beschreibender Titel für das Kunstwerk.</t>
+  </si>
+  <si>
+    <t>Hier erscheinen die Namen der Beteiligten, die für die Schaffung des Kunstwerks verantwortlich sind. Sind diese nicht überliefert, wird dies aktuell mit «Standardkünstler» zum Ausdruck gebracht.</t>
+  </si>
+  <si>
+    <t>Die geografischen Bezüge nehmen mehrheitlich Bezug auf den Herkunftsort des Kunstwerks. Wird explizit zwischen Herkunftsort und anderen Orten unterschieden, ist dies kenntlich gemacht.</t>
+  </si>
+  <si>
+    <t>Die Datierung beschreibt den Zeitpunkt oder Zeitraum der Herstellung des Kunstwerks. Ist ein anderer Zeitpunkt oder Zeitraum als der der Herstellung gemeint, wird dies kenntlich gemacht.</t>
+  </si>
+  <si>
+    <t>Die Masse beschreiben mehrheitlich die Textilfläche. Andere Masse werden kenntlich gemacht.</t>
+  </si>
+  <si>
+    <t>Verwendete Materialien und Techniken werden hintereinander aufgeführt, getrennt durch ein Semikolon.</t>
+  </si>
+  <si>
+    <t>Das Feld Sammlung gibt den oder die letzte(n) Vorbesitzer/in(nen) an und verweist darauf, dass sich weitere Kunstwerke dieser Person(en) in der Sammlung des Museums Rietberg befinden.</t>
+  </si>
+  <si>
+    <t>Aus der Creditline lässt sich ableiten, unter welchen Erwerbsumständen sich das Kunstwerk am Museum Rietberg befindet. In vielen Fällen wird dabei auch die oder der Vorbesitzer/in genannt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Provenienz widerspiegelt den aktuellen Kenntnisstand in Hinblick auf die Herkunftsgeschichte des Kunstwerks. </t>
+  </si>
+  <si>
+    <t>Die Kurzbeschreibung liefert zusätzliche Informationen zum Kunstwerk.</t>
+  </si>
+  <si>
+    <t>Unter Literaturverweis werden schriftliche Quellen aufgeführt, welche zusätzliche Informationen zum Kunstwerk beinhalten.</t>
+  </si>
+  <si>
+    <t>Der Bildnachweis gibt Aufschluss über die Rechteinhaber/innen in Hinblick auf die Fotografie des Kunstwerks.</t>
+  </si>
+  <si>
+    <t>Die Referenz zur Bilddatei erfolgt über den Dateinamen. Die Zip-Datei enthält zum Teil zusätzliche Ansichten eines Kunstwerks, diese werden jeweils durch den Suffix Underscore 1, 2, 3 etc. ausgewiesen.</t>
   </si>
 </sst>
 </file>
@@ -1450,15 +1499,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
+      <color theme="7" tint="0.59999389629810485"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1553,7 +1601,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
@@ -1663,10 +1711,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1919,25 +1964,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5" style="11" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="66.875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="53.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="66.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="53.58203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="8.75" style="5" customWidth="1"/>
-    <col min="6" max="6" width="88.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="50.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="88.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="50.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="255.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
@@ -1960,7 +2005,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
@@ -1978,7 +2023,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="312" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>54</v>
       </c>
@@ -1989,14 +2034,14 @@
         <v>14</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
@@ -2014,7 +2059,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
@@ -2030,7 +2075,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>25</v>
       </c>
@@ -2048,7 +2093,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>31</v>
       </c>
@@ -2066,7 +2111,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -2084,7 +2129,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>33</v>
       </c>
@@ -2102,7 +2147,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>34</v>
       </c>
@@ -2118,7 +2163,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>35</v>
       </c>
@@ -2136,7 +2181,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -2154,7 +2199,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>38</v>
       </c>
@@ -2172,7 +2217,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>39</v>
       </c>
@@ -2183,14 +2228,14 @@
         <v>14</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>49</v>
       </c>
@@ -2208,7 +2253,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>52</v>
       </c>
@@ -2226,7 +2271,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="35" t="s">
         <v>131</v>
       </c>
@@ -2236,22 +2281,22 @@
       <c r="C17" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="40" t="s">
-        <v>101</v>
+      <c r="D17" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="3"/>
       <c r="C18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>37</v>
       </c>
@@ -2264,7 +2309,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
         <v>11</v>
       </c>
@@ -2274,15 +2319,15 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="137.5" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>190</v>
+      <c r="B21" s="39" t="s">
+        <v>204</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="7"/>
@@ -2290,15 +2335,15 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="43" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="22" t="s">
-        <v>191</v>
+      <c r="B22" s="39" t="s">
+        <v>205</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="7"/>
@@ -2306,52 +2351,52 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="22" t="s">
-        <v>192</v>
+      <c r="B23" s="39" t="s">
+        <v>206</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>175</v>
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="25" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="22" t="s">
-        <v>193</v>
+      <c r="B24" s="39" t="s">
+        <v>207</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D25" s="24"/>
       <c r="E25" s="7"/>
       <c r="F25" s="24"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="1"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="1"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2359,7 +2404,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>29</v>
       </c>
@@ -2377,7 +2422,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" s="13" t="s">
         <v>26</v>
@@ -2393,323 +2438,338 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>177</v>
+        <v>218</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>186</v>
+        <v>222</v>
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>180</v>
+        <v>223</v>
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" s="4" customFormat="1" ht="50" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B42" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="C42" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="C42" s="22" t="s">
-        <v>187</v>
-      </c>
       <c r="D42" s="22" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>188</v>
+        <v>228</v>
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B44" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="E44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" s="4" customFormat="1" ht="50" x14ac:dyDescent="0.3">
+      <c r="A45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="C44" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="D44" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="E44" s="7"/>
-    </row>
-    <row r="45" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="11"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="7"/>
+      <c r="C45" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>229</v>
+      </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A46" s="11"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A47" s="11"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A48" s="11"/>
-      <c r="B48" s="3" t="s">
-        <v>167</v>
-      </c>
+      <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:6" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A49" s="11"/>
-      <c r="B49" s="3"/>
+      <c r="B49" s="3" t="s">
+        <v>167</v>
+      </c>
       <c r="C49" s="3"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A50" s="11"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
-      <c r="F50" s="4"/>
-    </row>
-    <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B51" s="13" t="s">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" ht="25" x14ac:dyDescent="0.3">
+      <c r="B52" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C52" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D51" s="13"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="8" t="s">
+      <c r="D52" s="13"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="8" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>161</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D53" s="12"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>165</v>
+      </c>
       <c r="D54" s="12"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.98425196850393704" bottom="0.59055118110236227" header="0.39370078740157483" footer="0.27559055118110237"/>
@@ -2725,131 +2785,131 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.375" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.25" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.375" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.375" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.875" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.625" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.375" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.58203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.58203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.08203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.58203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.75" style="25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.625" style="25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.875" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.58203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" style="25" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A17" s="31" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A18" s="31" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A19" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="36" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
         <v>130</v>
       </c>
@@ -2871,14 +2931,14 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="5.625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="5.58203125" style="25" customWidth="1"/>
     <col min="3" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>72</v>
       </c>
@@ -2886,27 +2946,27 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>73</v>
       </c>
@@ -2914,12 +2974,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
         <v>130</v>
       </c>
@@ -2941,14 +3001,14 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.375" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.25" style="25" customWidth="1"/>
     <col min="3" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>72</v>
       </c>
@@ -2956,118 +3016,118 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A18" s="27"/>
     </row>
-    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A19" s="27"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A22" s="27"/>
     </row>
-    <row r="23" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
     </row>
-    <row r="24" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A24" s="27"/>
     </row>
-    <row r="25" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A25" s="27"/>
     </row>
-    <row r="26" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A26" s="27"/>
     </row>
-    <row r="27" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A27" s="27"/>
     </row>
   </sheetData>
@@ -3087,15 +3147,15 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="5.375" style="25" customWidth="1"/>
-    <col min="3" max="3" width="58.625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="58.58203125" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="11" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>72</v>
       </c>
@@ -3106,7 +3166,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>89</v>
       </c>
@@ -3118,7 +3178,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>90</v>
       </c>
@@ -3130,7 +3190,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>91</v>
       </c>
@@ -3142,7 +3202,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>92</v>
       </c>
@@ -3154,7 +3214,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>93</v>
       </c>
@@ -3166,7 +3226,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
         <v>94</v>
       </c>
@@ -3178,7 +3238,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A8" s="28" t="s">
         <v>95</v>
       </c>
@@ -3190,7 +3250,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>96</v>
       </c>
@@ -3202,7 +3262,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>97</v>
       </c>
@@ -3214,7 +3274,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>98</v>
       </c>
@@ -3226,7 +3286,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>99</v>
       </c>
@@ -3238,7 +3298,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
         <v>100</v>
       </c>
@@ -3250,7 +3310,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>101</v>
       </c>
@@ -3262,7 +3322,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
         <v>102</v>
       </c>
@@ -3274,7 +3334,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
         <v>103</v>
       </c>
@@ -3286,12 +3346,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="33" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A22" s="34" t="s">
         <v>130</v>
       </c>
@@ -3308,6 +3368,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008CBAF0EEED2F5B4AB4463B97C2AD2B71" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d2bc9691d179cb44d4ba77bdf8fcfb4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c4a6dd5ef775a5269b08f7de37f93f">
     <xsd:element name="properties">
@@ -3421,22 +3496,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3450,27 +3533,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4B3AD83-9986-4E71-995F-A94C1CED6EB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update field name in metadata
</commit_message>
<xml_diff>
--- a/automation/mrz/Meta_Patolu.xlsx
+++ b/automation/mrz/Meta_Patolu.xlsx
@@ -1063,9 +1063,6 @@
     <t>kurzbeschreibung</t>
   </si>
   <si>
-    <t>bildunterschrift</t>
-  </si>
-  <si>
     <t>literatur</t>
   </si>
   <si>
@@ -1220,6 +1217,9 @@
   </si>
   <si>
     <t>Die Referenz zur Bilddatei erfolgt über den Dateinamen. Die Zip-Datei enthält zum Teil zusätzliche Ansichten eines Kunstwerks, diese werden jeweils durch den Suffix Underscore 1, 2, 3 etc. ausgewiesen.</t>
+  </si>
+  <si>
+    <t>bildnachweis</t>
   </si>
 </sst>
 </file>
@@ -1966,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="255.5" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2034,7 +2034,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
@@ -2324,10 +2324,10 @@
         <v>51</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="7"/>
@@ -2340,7 +2340,7 @@
         <v>51</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>187</v>
@@ -2356,10 +2356,10 @@
         <v>51</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>175</v>
@@ -2371,10 +2371,10 @@
         <v>51</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="7"/>
@@ -2449,7 +2449,7 @@
         <v>181</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="4" t="s">
@@ -2467,7 +2467,7 @@
         <v>178</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="4" t="s">
@@ -2482,10 +2482,10 @@
         <v>190</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="4" t="s">
@@ -2503,7 +2503,7 @@
         <v>177</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E34" s="7"/>
     </row>
@@ -2518,7 +2518,7 @@
         <v>182</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E35" s="7"/>
     </row>
@@ -2533,7 +2533,7 @@
         <v>183</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E36" s="7"/>
     </row>
@@ -2548,7 +2548,7 @@
         <v>185</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E37" s="7"/>
     </row>
@@ -2563,7 +2563,7 @@
         <v>179</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E38" s="7"/>
     </row>
@@ -2578,7 +2578,7 @@
         <v>180</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E39" s="7"/>
     </row>
@@ -2593,7 +2593,7 @@
         <v>184</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E40" s="7"/>
     </row>
@@ -2608,7 +2608,7 @@
         <v>186</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E41" s="7"/>
     </row>
@@ -2617,13 +2617,13 @@
         <v>30</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E42" s="7"/>
     </row>
@@ -2632,13 +2632,13 @@
         <v>30</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>199</v>
+        <v>229</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E43" s="7"/>
     </row>
@@ -2647,13 +2647,13 @@
         <v>30</v>
       </c>
       <c r="B44" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C44" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="D44" s="22" t="s">
         <v>214</v>
-      </c>
-      <c r="D44" s="22" t="s">
-        <v>215</v>
       </c>
       <c r="E44" s="7"/>
     </row>
@@ -2665,10 +2665,10 @@
         <v>159</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E45" s="7"/>
     </row>
@@ -3368,21 +3368,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008CBAF0EEED2F5B4AB4463B97C2AD2B71" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="d2bc9691d179cb44d4ba77bdf8fcfb4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66c4a6dd5ef775a5269b08f7de37f93f">
     <xsd:element name="properties">
@@ -3496,17 +3481,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3520,17 +3521,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F33FC2A8-E9AF-48AF-8CDC-2C0CCE48C45D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6056489-A7A4-4445-AFC5-87E5586E5E93}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>